<commit_message>
Save Entity on Database
</commit_message>
<xml_diff>
--- a/UnitTest/output/CreateWithWorksheets.xlsx
+++ b/UnitTest/output/CreateWithWorksheets.xlsx
@@ -5,34 +5,37 @@
     <workbookView/>
   </bookViews>
   <sheets>
-    <sheet name="My Data" sheetId="1" r:id="rId1"/>
+    <sheet name="People" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Name</t>
   </si>
   <si>
-    <t>Birthdate</t>
+    <t>BirthDate</t>
   </si>
   <si>
     <t>John</t>
   </si>
   <si>
-    <t>18/12/2002</t>
+    <t>18/12/2002 00:00:00</t>
   </si>
   <si>
     <t>James</t>
   </si>
   <si>
-    <t>19/03/2000</t>
+    <t>19/03/2000 00:00:00</t>
   </si>
   <si>
     <t>Jonathan</t>
+  </si>
+  <si>
+    <t>20/05/1999 00:00:00</t>
   </si>
 </sst>
 </file>
@@ -113,6 +116,9 @@
       <c r="A4" s="0" t="s">
         <v>6</v>
       </c>
+      <c r="B4" s="0" t="s">
+        <v>7</v>
+      </c>
     </row>
   </sheetData>
   <headerFooter/>

</xml_diff>